<commit_message>
update code for t8
</commit_message>
<xml_diff>
--- a/Báo cáo/0_HỆ THỐNG/Danh sách khách hàng/Danh sách khách hàng còn dư nợ tại HỆ THỐNG.xlsx
+++ b/Báo cáo/0_HỆ THỐNG/Danh sách khách hàng/Danh sách khách hàng còn dư nợ tại HỆ THỐNG.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,25 +480,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lâm Minh Ngọc</t>
+          <t>ngọc hân</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v/>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0766931276</t>
-        </is>
+      <c r="F2" t="n">
+        <v/>
       </c>
       <c r="G2" t="n">
         <v/>
@@ -507,10 +505,10 @@
         <v/>
       </c>
       <c r="I2" t="n">
-        <v>10000000</v>
+        <v>35000000</v>
       </c>
       <c r="J2" t="n">
-        <v>10000000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="3">
@@ -520,16 +518,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nguyễn thị mỹ trinh</t>
+          <t>Lâm Minh Ngọc</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -537,7 +535,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0865927791</t>
+          <t>0766931276</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -547,10 +545,10 @@
         <v/>
       </c>
       <c r="I3" t="n">
-        <v>22000000</v>
+        <v>10000000</v>
       </c>
       <c r="J3" t="n">
-        <v>7000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="4">
@@ -560,16 +558,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Chị vui</t>
+          <t>nguyễn thị mỹ trinh</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -577,7 +575,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>094990449</t>
+          <t>0865927791</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -587,10 +585,10 @@
         <v/>
       </c>
       <c r="I4" t="n">
-        <v>1000000</v>
+        <v>22000000</v>
       </c>
       <c r="J4" t="n">
-        <v>2000000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="5">
@@ -600,16 +598,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>353</v>
+        <v>371</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lê Thị Kiều</t>
+          <t>Chị vui</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -617,7 +615,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0907746583</t>
+          <t>094990449</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -627,10 +625,10 @@
         <v/>
       </c>
       <c r="I5" t="n">
-        <v>7500000</v>
+        <v>1000000</v>
       </c>
       <c r="J5" t="n">
-        <v>10500000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="6">
@@ -640,11 +638,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Nguyễn Ngọc My</t>
+          <t>Lê Thị Kiều</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -657,7 +655,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0325266431</t>
+          <t>0907746583</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -667,10 +665,10 @@
         <v/>
       </c>
       <c r="I6" t="n">
-        <v>32000000</v>
+        <v>7500000</v>
       </c>
       <c r="J6" t="n">
-        <v>3000000</v>
+        <v>10500000</v>
       </c>
     </row>
     <row r="7">
@@ -680,16 +678,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">nguyễn thị lệ trang </t>
+          <t>Nguyễn Ngọc My</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -697,7 +695,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0786070121</t>
+          <t>0325266431</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -707,10 +705,10 @@
         <v/>
       </c>
       <c r="I7" t="n">
-        <v>25000000</v>
+        <v>32000000</v>
       </c>
       <c r="J7" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="8">
@@ -720,16 +718,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Nguyễn Phương Thuý</t>
+          <t xml:space="preserve">nguyễn thị lệ trang </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -737,7 +735,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0787996460</t>
+          <t>0786070121</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -747,10 +745,10 @@
         <v/>
       </c>
       <c r="I8" t="n">
-        <v>1500000</v>
+        <v>25000000</v>
       </c>
       <c r="J8" t="n">
-        <v>300000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="9">
@@ -760,16 +758,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Huỳnh thị bé sáu</t>
+          <t>Nguyễn Phương Thuý</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -777,7 +775,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0912122976</t>
+          <t>0787996460</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -787,10 +785,10 @@
         <v/>
       </c>
       <c r="I9" t="n">
-        <v>9000000</v>
+        <v>1500000</v>
       </c>
       <c r="J9" t="n">
-        <v>2500000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="10">
@@ -800,23 +798,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>thuý vân</t>
+          <t>Huỳnh thị bé sáu</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v/>
       </c>
-      <c r="F10" t="n">
-        <v/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0912122976</t>
+        </is>
       </c>
       <c r="G10" t="n">
         <v/>
@@ -825,10 +825,10 @@
         <v/>
       </c>
       <c r="I10" t="n">
-        <v>15000000</v>
+        <v>9000000</v>
       </c>
       <c r="J10" t="n">
-        <v>20000000</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="11">
@@ -838,25 +838,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ngô Xuân Nhi</t>
+          <t>thuý vân</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v/>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0868883621</t>
-        </is>
+      <c r="F11" t="n">
+        <v/>
       </c>
       <c r="G11" t="n">
         <v/>
@@ -865,10 +863,10 @@
         <v/>
       </c>
       <c r="I11" t="n">
-        <v>9500000</v>
+        <v>15000000</v>
       </c>
       <c r="J11" t="n">
-        <v>8500000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="12">
@@ -878,23 +876,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>nguyễn thị hân</t>
+          <t>Ngô Xuân Nhi</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E12" t="n">
         <v/>
       </c>
-      <c r="F12" t="n">
-        <v/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0868883621</t>
+        </is>
       </c>
       <c r="G12" t="n">
         <v/>
@@ -903,10 +903,10 @@
         <v/>
       </c>
       <c r="I12" t="n">
-        <v>4000000</v>
+        <v>9500000</v>
       </c>
       <c r="J12" t="n">
-        <v>3000000</v>
+        <v>8500000</v>
       </c>
     </row>
     <row r="13">
@@ -916,25 +916,23 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hoàng Thị Thu Vân</t>
+          <t>nguyễn thị hân</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E13" t="n">
         <v/>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>0761880789</t>
-        </is>
+      <c r="F13" t="n">
+        <v/>
       </c>
       <c r="G13" t="n">
         <v/>
@@ -943,10 +941,10 @@
         <v/>
       </c>
       <c r="I13" t="n">
-        <v>1000000</v>
+        <v>4000000</v>
       </c>
       <c r="J13" t="n">
-        <v>500000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="14">
@@ -956,11 +954,11 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Hồng Nho</t>
+          <t>Hoàng Thị Thu Vân</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -973,7 +971,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0971073757</t>
+          <t>0761880789</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -983,10 +981,10 @@
         <v/>
       </c>
       <c r="I14" t="n">
-        <v>14730000</v>
+        <v>1000000</v>
       </c>
       <c r="J14" t="n">
-        <v>3000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="15">
@@ -996,23 +994,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">nguyễn hồng tơ </t>
+          <t>Nguyễn Thị Hồng Nho</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v/>
       </c>
-      <c r="F15" t="n">
-        <v/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0971073757</t>
+        </is>
       </c>
       <c r="G15" t="n">
         <v/>
@@ -1021,10 +1021,10 @@
         <v/>
       </c>
       <c r="I15" t="n">
-        <v>2850000</v>
+        <v>14730000</v>
       </c>
       <c r="J15" t="n">
-        <v>5600000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="16">
@@ -1034,11 +1034,11 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>chị lan</t>
+          <t xml:space="preserve">nguyễn hồng tơ </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1049,10 +1049,8 @@
       <c r="E16" t="n">
         <v/>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>032781693</t>
-        </is>
+      <c r="F16" t="n">
+        <v/>
       </c>
       <c r="G16" t="n">
         <v/>
@@ -1061,10 +1059,10 @@
         <v/>
       </c>
       <c r="I16" t="n">
-        <v>10000000</v>
+        <v>2850000</v>
       </c>
       <c r="J16" t="n">
-        <v>15000000</v>
+        <v>5600000</v>
       </c>
     </row>
     <row r="17">
@@ -1074,11 +1072,11 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>pola</t>
+          <t>chị lan</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1089,8 +1087,10 @@
       <c r="E17" t="n">
         <v/>
       </c>
-      <c r="F17" t="n">
-        <v/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>032781693</t>
+        </is>
       </c>
       <c r="G17" t="n">
         <v/>
@@ -1099,10 +1099,10 @@
         <v/>
       </c>
       <c r="I17" t="n">
-        <v>22000000</v>
+        <v>10000000</v>
       </c>
       <c r="J17" t="n">
-        <v>21000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="18">
@@ -1112,11 +1112,11 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">nguyễn thị sen </t>
+          <t>pola</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1127,10 +1127,8 @@
       <c r="E18" t="n">
         <v/>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>0852054955</t>
-        </is>
+      <c r="F18" t="n">
+        <v/>
       </c>
       <c r="G18" t="n">
         <v/>
@@ -1139,10 +1137,10 @@
         <v/>
       </c>
       <c r="I18" t="n">
-        <v>5000000</v>
+        <v>22000000</v>
       </c>
       <c r="J18" t="n">
-        <v>2000000</v>
+        <v>21000000</v>
       </c>
     </row>
     <row r="19">
@@ -1152,11 +1150,11 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">chị ngọc </t>
+          <t xml:space="preserve">nguyễn thị sen </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1167,8 +1165,10 @@
       <c r="E19" t="n">
         <v/>
       </c>
-      <c r="F19" t="n">
-        <v/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0852054955</t>
+        </is>
       </c>
       <c r="G19" t="n">
         <v/>
@@ -1177,10 +1177,10 @@
         <v/>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J19" t="n">
-        <v>7000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="20">
@@ -1190,11 +1190,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">chị liên </t>
+          <t xml:space="preserve">chị ngọc </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>10500000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="21">
@@ -1228,11 +1228,11 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">chị trúc </t>
+          <t xml:space="preserve">chị liên </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>15000000</v>
+        <v>10500000</v>
       </c>
     </row>
     <row r="22">
@@ -1266,11 +1266,11 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>nhân nhân</t>
+          <t xml:space="preserve">chị trúc </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>7000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="23">
@@ -1304,11 +1304,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>khanh ktv cũ</t>
+          <t>nhân nhân</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>7900000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="24">
@@ -1342,11 +1342,11 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>nguyễn thị ánh tuyết</t>
+          <t>khanh ktv cũ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>16500000</v>
+        <v>7900000</v>
       </c>
     </row>
     <row r="25">
@@ -1380,25 +1380,23 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Mai thị nương</t>
+          <t>nguyễn thị ánh tuyết</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E25" t="n">
         <v/>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>0975352074</t>
-        </is>
+      <c r="F25" t="n">
+        <v/>
       </c>
       <c r="G25" t="n">
         <v/>
@@ -1407,10 +1405,10 @@
         <v/>
       </c>
       <c r="I25" t="n">
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>1500000</v>
+        <v>16500000</v>
       </c>
     </row>
     <row r="26">
@@ -1420,16 +1418,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Phạm Trần Thuý Vi</t>
+          <t>Mai thị nương</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1437,7 +1435,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0974370797</t>
+          <t>0975352074</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1447,10 +1445,10 @@
         <v/>
       </c>
       <c r="I26" t="n">
-        <v>10000000</v>
+        <v>1500000</v>
       </c>
       <c r="J26" t="n">
-        <v>5000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="27">
@@ -1460,11 +1458,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Trần Thị Lan Trinh</t>
+          <t>Phạm Trần Thuý Vi</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1477,7 +1475,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0918667208</t>
+          <t>0974370797</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1500,11 +1498,11 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Nguyễn Hữu Dân</t>
+          <t>Trần Thị Lan Trinh</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1517,7 +1515,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0868586369</t>
+          <t>0918667208</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1527,10 +1525,10 @@
         <v/>
       </c>
       <c r="I28" t="n">
-        <v>2000000</v>
+        <v>10000000</v>
       </c>
       <c r="J28" t="n">
-        <v>500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="29">
@@ -1540,16 +1538,16 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Võ thị nga</t>
+          <t>Nguyễn Hữu Dân</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1557,7 +1555,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0768862580</t>
+          <t>0868586369</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1567,10 +1565,10 @@
         <v/>
       </c>
       <c r="I29" t="n">
-        <v>5800000</v>
+        <v>2000000</v>
       </c>
       <c r="J29" t="n">
-        <v>1700000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="30">
@@ -1580,23 +1578,25 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Em My</t>
+          <t>Võ thị nga</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E30" t="n">
         <v/>
       </c>
-      <c r="F30" t="n">
-        <v/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>0768862580</t>
+        </is>
       </c>
       <c r="G30" t="n">
         <v/>
@@ -1605,10 +1605,10 @@
         <v/>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>5800000</v>
       </c>
       <c r="J30" t="n">
-        <v>400000</v>
+        <v>1700000</v>
       </c>
     </row>
     <row r="31">
@@ -1618,11 +1618,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Lâm t.dân</t>
+          <t>Em My</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1643,10 +1643,10 @@
         <v/>
       </c>
       <c r="I31" t="n">
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>500000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="32">
@@ -1656,11 +1656,11 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>chị Na</t>
+          <t>Lâm t.dân</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1681,10 +1681,10 @@
         <v/>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="J32" t="n">
-        <v>5000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="33">
@@ -1694,11 +1694,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">em Tuyền </t>
+          <t>chị Na</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1709,10 +1709,8 @@
       <c r="E33" t="n">
         <v/>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>0369473448</t>
-        </is>
+      <c r="F33" t="n">
+        <v/>
       </c>
       <c r="G33" t="n">
         <v/>
@@ -1721,7 +1719,7 @@
         <v/>
       </c>
       <c r="I33" t="n">
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
         <v>5000000</v>
@@ -1734,11 +1732,11 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>em Trinh</t>
+          <t xml:space="preserve">em Tuyền </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1749,8 +1747,10 @@
       <c r="E34" t="n">
         <v/>
       </c>
-      <c r="F34" t="n">
-        <v/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0369473448</t>
+        </is>
       </c>
       <c r="G34" t="n">
         <v/>
@@ -1762,7 +1762,7 @@
         <v>5000000</v>
       </c>
       <c r="J34" t="n">
-        <v>3386000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="35">
@@ -1772,25 +1772,23 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Em gấm</t>
+          <t>em Trinh</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E35" t="n">
         <v/>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>0764666615</t>
-        </is>
+      <c r="F35" t="n">
+        <v/>
       </c>
       <c r="G35" t="n">
         <v/>
@@ -1799,10 +1797,10 @@
         <v/>
       </c>
       <c r="I35" t="n">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="J35" t="n">
-        <v>15000000</v>
+        <v>3386000</v>
       </c>
     </row>
     <row r="36">
@@ -1812,16 +1810,16 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">đỗ bảo loan </t>
+          <t>Em gấm</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1829,7 +1827,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>8947126536</t>
+          <t>0764666615</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1839,10 +1837,10 @@
         <v/>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="J36" t="n">
-        <v>4000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="37">
@@ -1852,11 +1850,11 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>phalla</t>
+          <t xml:space="preserve">đỗ bảo loan </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1867,8 +1865,10 @@
       <c r="E37" t="n">
         <v/>
       </c>
-      <c r="F37" t="n">
-        <v/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>8947126536</t>
+        </is>
       </c>
       <c r="G37" t="n">
         <v/>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>25000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="38">
@@ -1890,25 +1890,23 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Nguyễn Đoàn Tuyết Nhung</t>
+          <t>phalla</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E38" t="n">
         <v/>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>0968119924</t>
-        </is>
+      <c r="F38" t="n">
+        <v/>
       </c>
       <c r="G38" t="n">
         <v/>
@@ -1917,10 +1915,10 @@
         <v/>
       </c>
       <c r="I38" t="n">
-        <v>26000000</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>9000000</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="39">
@@ -1930,11 +1928,11 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Trần Thị Phượng Hằng</t>
+          <t>Nguyễn Đoàn Tuyết Nhung</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1947,7 +1945,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0797571132</t>
+          <t>0968119924</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1957,10 +1955,10 @@
         <v/>
       </c>
       <c r="I39" t="n">
-        <v>24300000</v>
+        <v>26000000</v>
       </c>
       <c r="J39" t="n">
-        <v>3000000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="40">
@@ -1970,11 +1968,11 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Phan Yến Nhi</t>
+          <t>Trần Thị Phượng Hằng</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1987,7 +1985,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0799675368</t>
+          <t>0797571132</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1997,10 +1995,10 @@
         <v/>
       </c>
       <c r="I40" t="n">
-        <v>4000000</v>
+        <v>24300000</v>
       </c>
       <c r="J40" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="41">
@@ -2010,11 +2008,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Tuyết Hiếu</t>
+          <t>Phan Yến Nhi</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2027,7 +2025,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0868748958</t>
+          <t>0799675368</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -2037,10 +2035,10 @@
         <v/>
       </c>
       <c r="I41" t="n">
-        <v>10000000</v>
+        <v>4000000</v>
       </c>
       <c r="J41" t="n">
-        <v>18000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="42">
@@ -2050,24 +2048,24 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sơn thị chuol</t>
+          <t>Nguyễn Thị Tuyết Hiếu</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>9417002720</v>
+        <v/>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0374112377</t>
+          <t>0868748958</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -2077,10 +2075,10 @@
         <v/>
       </c>
       <c r="I42" t="n">
-        <v>25000000</v>
+        <v>10000000</v>
       </c>
       <c r="J42" t="n">
-        <v>12000000</v>
+        <v>18000000</v>
       </c>
     </row>
     <row r="43">
@@ -2090,24 +2088,24 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lâm Nhật Thái</t>
+          <t>sơn thị chuol</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v/>
+        <v>9417002720</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0946327273</t>
+          <t>0374112377</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -2117,10 +2115,10 @@
         <v/>
       </c>
       <c r="I43" t="n">
-        <v>8000000</v>
+        <v>25000000</v>
       </c>
       <c r="J43" t="n">
-        <v>5000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="44">
@@ -2130,11 +2128,11 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Phan Mỹ Điền</t>
+          <t>Lâm Nhật Thái</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2147,7 +2145,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0847413423</t>
+          <t>0946327273</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -2157,10 +2155,10 @@
         <v/>
       </c>
       <c r="I44" t="n">
-        <v>16000000</v>
+        <v>8000000</v>
       </c>
       <c r="J44" t="n">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="45">
@@ -2170,16 +2168,16 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Chị Tâm</t>
+          <t>Phan Mỹ Điền</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2187,7 +2185,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0396237229</t>
+          <t>0847413423</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2197,10 +2195,10 @@
         <v/>
       </c>
       <c r="I45" t="n">
+        <v>16000000</v>
+      </c>
+      <c r="J45" t="n">
         <v>4000000</v>
-      </c>
-      <c r="J45" t="n">
-        <v>2000000</v>
       </c>
     </row>
     <row r="46">
@@ -2210,11 +2208,11 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Hồ thị Kim thoa</t>
+          <t>Chị Tâm</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2227,7 +2225,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0964414150</t>
+          <t>0396237229</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2237,10 +2235,10 @@
         <v/>
       </c>
       <c r="I46" t="n">
-        <v>8000000</v>
+        <v>4000000</v>
       </c>
       <c r="J46" t="n">
-        <v>17000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="47">
@@ -2250,11 +2248,11 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Chị diễm</t>
+          <t>Hồ thị Kim thoa</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2267,7 +2265,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0918665056</t>
+          <t>0964414150</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2277,10 +2275,10 @@
         <v/>
       </c>
       <c r="I47" t="n">
-        <v>1000000</v>
+        <v>8000000</v>
       </c>
       <c r="J47" t="n">
-        <v>1300000</v>
+        <v>17000000</v>
       </c>
     </row>
     <row r="48">
@@ -2290,16 +2288,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Trần Thị Cẩm Hồng</t>
+          <t>Chị diễm</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -2307,7 +2305,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0939773382</t>
+          <t>0918665056</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2317,10 +2315,10 @@
         <v/>
       </c>
       <c r="I48" t="n">
-        <v>15000000</v>
+        <v>1000000</v>
       </c>
       <c r="J48" t="n">
-        <v>5000000</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="49">
@@ -2330,11 +2328,11 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Trần Nguyễn Yến Linh</t>
+          <t>Trần Thị Cẩm Hồng</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2347,7 +2345,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0777004897</t>
+          <t>0939773382</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2357,10 +2355,10 @@
         <v/>
       </c>
       <c r="I49" t="n">
-        <v>10000000</v>
+        <v>15000000</v>
       </c>
       <c r="J49" t="n">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="50">
@@ -2370,23 +2368,25 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Em Như + Mẹ</t>
+          <t>Trần Nguyễn Yến Linh</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E50" t="n">
         <v/>
       </c>
-      <c r="F50" t="n">
-        <v/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0777004897</t>
+        </is>
       </c>
       <c r="G50" t="n">
         <v/>
@@ -2395,10 +2395,10 @@
         <v/>
       </c>
       <c r="I50" t="n">
-        <v>53000000</v>
+        <v>10000000</v>
       </c>
       <c r="J50" t="n">
-        <v>7000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="51">
@@ -2408,25 +2408,23 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Mai Bảo Thi</t>
+          <t>Em Như + Mẹ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E51" t="n">
         <v/>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>0982030044</t>
-        </is>
+      <c r="F51" t="n">
+        <v/>
       </c>
       <c r="G51" t="n">
         <v/>
@@ -2435,10 +2433,10 @@
         <v/>
       </c>
       <c r="I51" t="n">
-        <v>10000000</v>
+        <v>53000000</v>
       </c>
       <c r="J51" t="n">
-        <v>10000000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="52">
@@ -2448,11 +2446,11 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kim Ngân</t>
+          <t>Mai Bảo Thi</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2463,8 +2461,10 @@
       <c r="E52" t="n">
         <v/>
       </c>
-      <c r="F52" t="n">
-        <v/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>0982030044</t>
+        </is>
       </c>
       <c r="G52" t="n">
         <v/>
@@ -2473,10 +2473,10 @@
         <v/>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="J52" t="n">
-        <v>3000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="53">
@@ -2486,11 +2486,11 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Trần Thị Hồng Cẩm</t>
+          <t>Kim Ngân</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2511,10 +2511,10 @@
         <v/>
       </c>
       <c r="I53" t="n">
-        <v>22500000</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="54">
@@ -2524,11 +2524,11 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Thuỳ Nhiên</t>
+          <t>Trần Thị Hồng Cẩm</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2549,10 +2549,10 @@
         <v/>
       </c>
       <c r="I54" t="n">
-        <v>500000</v>
+        <v>22500000</v>
       </c>
       <c r="J54" t="n">
-        <v>1500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="55">
@@ -2562,25 +2562,23 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Nhi</t>
+          <t>Thuỳ Nhiên</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E55" t="n">
         <v/>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>0387888961</t>
-        </is>
+      <c r="F55" t="n">
+        <v/>
       </c>
       <c r="G55" t="n">
         <v/>
@@ -2589,10 +2587,10 @@
         <v/>
       </c>
       <c r="I55" t="n">
-        <v>5000000</v>
+        <v>500000</v>
       </c>
       <c r="J55" t="n">
-        <v>12000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="56">
@@ -2602,11 +2600,11 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>em thuý</t>
+          <t>Nguyễn Thị Nhi</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2617,8 +2615,10 @@
       <c r="E56" t="n">
         <v/>
       </c>
-      <c r="F56" t="n">
-        <v/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0387888961</t>
+        </is>
       </c>
       <c r="G56" t="n">
         <v/>
@@ -2627,10 +2627,10 @@
         <v/>
       </c>
       <c r="I56" t="n">
-        <v>15000000</v>
+        <v>5000000</v>
       </c>
       <c r="J56" t="n">
-        <v>5000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="57">
@@ -2640,11 +2640,11 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Tú Trâm</t>
+          <t>em thuý</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2678,11 +2678,11 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>chị Dung</t>
+          <t>Tú Trâm</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2693,10 +2693,8 @@
       <c r="E58" t="n">
         <v/>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>0373886477</t>
-        </is>
+      <c r="F58" t="n">
+        <v/>
       </c>
       <c r="G58" t="n">
         <v/>
@@ -2705,10 +2703,10 @@
         <v/>
       </c>
       <c r="I58" t="n">
-        <v>85000000</v>
+        <v>15000000</v>
       </c>
       <c r="J58" t="n">
-        <v>30000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="59">
@@ -2718,23 +2716,25 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Cô phương</t>
+          <t>chị Dung</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E59" t="n">
         <v/>
       </c>
-      <c r="F59" t="n">
-        <v/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0373886477</t>
+        </is>
       </c>
       <c r="G59" t="n">
         <v/>
@@ -2743,10 +2743,10 @@
         <v/>
       </c>
       <c r="I59" t="n">
-        <v>2000000</v>
+        <v>85000000</v>
       </c>
       <c r="J59" t="n">
-        <v>500000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="60">
@@ -2756,11 +2756,11 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Cô tú</t>
+          <t>Cô phương</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2781,10 +2781,10 @@
         <v/>
       </c>
       <c r="I60" t="n">
-        <v>2500000</v>
+        <v>2000000</v>
       </c>
       <c r="J60" t="n">
-        <v>2000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="61">
@@ -2794,11 +2794,11 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Chị Ngoan</t>
+          <t>Cô tú</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2819,10 +2819,10 @@
         <v/>
       </c>
       <c r="I61" t="n">
-        <v>10000000</v>
+        <v>2500000</v>
       </c>
       <c r="J61" t="n">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="62">
@@ -2832,11 +2832,11 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Em Xuyên</t>
+          <t>Chị Ngoan</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2857,10 +2857,10 @@
         <v/>
       </c>
       <c r="I62" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="J62" t="n">
         <v>5000000</v>
-      </c>
-      <c r="J62" t="n">
-        <v>6000000</v>
       </c>
     </row>
     <row r="63">
@@ -2870,11 +2870,11 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>em bang</t>
+          <t>Em Xuyên</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2895,10 +2895,10 @@
         <v/>
       </c>
       <c r="I63" t="n">
-        <v>36900000</v>
+        <v>5000000</v>
       </c>
       <c r="J63" t="n">
-        <v>14000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="64">
@@ -2908,16 +2908,16 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>bé bảy</t>
+          <t>em bang</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -2933,10 +2933,10 @@
         <v/>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>36900000</v>
       </c>
       <c r="J64" t="n">
-        <v>1000000</v>
+        <v>14000000</v>
       </c>
     </row>
     <row r="65">
@@ -2946,11 +2946,11 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Khải MX</t>
+          <t>bé bảy</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2971,10 +2971,10 @@
         <v/>
       </c>
       <c r="I65" t="n">
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="66">
@@ -2984,11 +2984,11 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>My</t>
+          <t>Khải MX</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -3009,10 +3009,10 @@
         <v/>
       </c>
       <c r="I66" t="n">
-        <v>18900000</v>
+        <v>10000000</v>
       </c>
       <c r="J66" t="n">
-        <v>7200000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="67">
@@ -3022,11 +3022,11 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Duyên</t>
+          <t>My</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3047,10 +3047,10 @@
         <v/>
       </c>
       <c r="I67" t="n">
-        <v>10000000</v>
+        <v>18900000</v>
       </c>
       <c r="J67" t="n">
-        <v>5000000</v>
+        <v>7200000</v>
       </c>
     </row>
     <row r="68">
@@ -3060,11 +3060,11 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>c phép khểnh</t>
+          <t>Duyên</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3085,10 +3085,10 @@
         <v/>
       </c>
       <c r="I68" t="n">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="J68" t="n">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="69">
@@ -3098,16 +3098,16 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>trần kiều trinh</t>
+          <t>c phép khểnh</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -3123,10 +3123,10 @@
         <v/>
       </c>
       <c r="I69" t="n">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>4000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="70">
@@ -3136,11 +3136,11 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>lê hoàng phúc</t>
+          <t>trần kiều trinh</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3151,10 +3151,8 @@
       <c r="E70" t="n">
         <v/>
       </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>TN-89</t>
-        </is>
+      <c r="F70" t="n">
+        <v/>
       </c>
       <c r="G70" t="n">
         <v/>
@@ -3163,10 +3161,10 @@
         <v/>
       </c>
       <c r="I70" t="n">
-        <v>3000000</v>
+        <v>15000000</v>
       </c>
       <c r="J70" t="n">
-        <v>27000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="71">
@@ -3176,11 +3174,11 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>anh tiến</t>
+          <t>lê hoàng phúc</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3191,8 +3189,10 @@
       <c r="E71" t="n">
         <v/>
       </c>
-      <c r="F71" t="n">
-        <v/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>TN-89</t>
+        </is>
       </c>
       <c r="G71" t="n">
         <v/>
@@ -3201,10 +3201,10 @@
         <v/>
       </c>
       <c r="I71" t="n">
-        <v>10000000</v>
+        <v>3000000</v>
       </c>
       <c r="J71" t="n">
-        <v>3000000</v>
+        <v>27000000</v>
       </c>
     </row>
     <row r="72">
@@ -3214,11 +3214,11 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Phạm Thanh Tiến</t>
+          <t>anh tiến</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v/>
       </c>
       <c r="I72" t="n">
-        <v>2000000</v>
+        <v>10000000</v>
       </c>
       <c r="J72" t="n">
-        <v>23000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="73">
@@ -3252,11 +3252,11 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Quỳnh Như</t>
+          <t>Phạm Thanh Tiến</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3265,12 +3265,10 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>89197014107</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>0822323252</t>
-        </is>
+        <v/>
+      </c>
+      <c r="F73" t="n">
+        <v/>
       </c>
       <c r="G73" t="n">
         <v/>
@@ -3279,10 +3277,10 @@
         <v/>
       </c>
       <c r="I73" t="n">
-        <v>25000000</v>
+        <v>2000000</v>
       </c>
       <c r="J73" t="n">
-        <v>24000000</v>
+        <v>23000000</v>
       </c>
     </row>
     <row r="74">
@@ -3292,11 +3290,11 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Mỹ Nhung</t>
+          <t>Nguyễn Thị Quỳnh Như</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3305,10 +3303,12 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v/>
-      </c>
-      <c r="F74" t="n">
-        <v/>
+        <v>89197014107</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>0822323252</t>
+        </is>
       </c>
       <c r="G74" t="n">
         <v/>
@@ -3317,10 +3317,10 @@
         <v/>
       </c>
       <c r="I74" t="n">
-        <v>4700000</v>
+        <v>25000000</v>
       </c>
       <c r="J74" t="n">
-        <v>20000000</v>
+        <v>24000000</v>
       </c>
     </row>
     <row r="75">
@@ -3330,11 +3330,11 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>thanh thảo</t>
+          <t>Mỹ Nhung</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3355,10 +3355,10 @@
         <v/>
       </c>
       <c r="I75" t="n">
-        <v>0</v>
+        <v>4700000</v>
       </c>
       <c r="J75" t="n">
-        <v>5000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="76">
@@ -3368,11 +3368,11 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>hoài hưng</t>
+          <t>thanh thảo</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3396,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>21000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="77">
@@ -3406,11 +3406,11 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Duyên</t>
+          <t>hoài hưng</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3421,10 +3421,8 @@
       <c r="E77" t="n">
         <v/>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>0767509572</t>
-        </is>
+      <c r="F77" t="n">
+        <v/>
       </c>
       <c r="G77" t="n">
         <v/>
@@ -3433,10 +3431,10 @@
         <v/>
       </c>
       <c r="I77" t="n">
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>28000000</v>
+        <v>21000000</v>
       </c>
     </row>
     <row r="78">
@@ -3446,11 +3444,11 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>chị Bỉ</t>
+          <t>Nguyễn Thị Duyên</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3461,8 +3459,10 @@
       <c r="E78" t="n">
         <v/>
       </c>
-      <c r="F78" t="n">
-        <v/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>0767509572</t>
+        </is>
       </c>
       <c r="G78" t="n">
         <v/>
@@ -3471,10 +3471,10 @@
         <v/>
       </c>
       <c r="I78" t="n">
-        <v>1200000</v>
+        <v>10000000</v>
       </c>
       <c r="J78" t="n">
-        <v>300000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="79">
@@ -3484,11 +3484,11 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Hồng Trang</t>
+          <t>chị Bỉ</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3509,10 +3509,10 @@
         <v/>
       </c>
       <c r="I79" t="n">
-        <v>4300000</v>
+        <v>1200000</v>
       </c>
       <c r="J79" t="n">
-        <v>29500000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="80">
@@ -3522,11 +3522,11 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>kim quyên</t>
+          <t>Nguyễn Thị Hồng Trang</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3547,10 +3547,10 @@
         <v/>
       </c>
       <c r="I80" t="n">
-        <v>4000000</v>
+        <v>4300000</v>
       </c>
       <c r="J80" t="n">
-        <v>6000000</v>
+        <v>29500000</v>
       </c>
     </row>
     <row r="81">
@@ -3560,11 +3560,11 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Nguyễn Thi Thức ( My )</t>
+          <t>kim quyên</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3575,10 +3575,8 @@
       <c r="E81" t="n">
         <v/>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>0332812716</t>
-        </is>
+      <c r="F81" t="n">
+        <v/>
       </c>
       <c r="G81" t="n">
         <v/>
@@ -3587,10 +3585,10 @@
         <v/>
       </c>
       <c r="I81" t="n">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
       <c r="J81" t="n">
-        <v>12000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="82">
@@ -3600,11 +3598,11 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>em tiên</t>
+          <t>Nguyễn Thi Thức ( My )</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3615,8 +3613,10 @@
       <c r="E82" t="n">
         <v/>
       </c>
-      <c r="F82" t="n">
-        <v/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>0332812716</t>
+        </is>
       </c>
       <c r="G82" t="n">
         <v/>
@@ -3625,10 +3625,10 @@
         <v/>
       </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>13000000</v>
       </c>
       <c r="J82" t="n">
-        <v>2000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="83">
@@ -3638,11 +3638,11 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>em Ái Mỹ</t>
+          <t>em tiên</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3666,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="84">
@@ -3676,11 +3676,11 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Trần Nguyễn Sang Sang</t>
+          <t>em Ái Mỹ</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3691,10 +3691,8 @@
       <c r="E84" t="n">
         <v/>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>0868277767</t>
-        </is>
+      <c r="F84" t="n">
+        <v/>
       </c>
       <c r="G84" t="n">
         <v/>
@@ -3703,10 +3701,10 @@
         <v/>
       </c>
       <c r="I84" t="n">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>12000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="85">
@@ -3716,11 +3714,11 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>em Trúc</t>
+          <t>Trần Nguyễn Sang Sang</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3731,8 +3729,10 @@
       <c r="E85" t="n">
         <v/>
       </c>
-      <c r="F85" t="n">
-        <v/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>0868277767</t>
+        </is>
       </c>
       <c r="G85" t="n">
         <v/>
@@ -3741,10 +3741,10 @@
         <v/>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="J85" t="n">
-        <v>1500000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="86">
@@ -3754,11 +3754,11 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Ngọc Hân 2</t>
+          <t>em Trúc</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>7000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="87">
@@ -3792,16 +3792,16 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>chị Lợi</t>
+          <t>Ngọc Hân 2</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>LONG XUYÊN</t>
+          <t>CẦN THƠ</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -3817,10 +3817,10 @@
         <v/>
       </c>
       <c r="I87" t="n">
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="J87" t="n">
-        <v>1500000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="88">
@@ -3830,11 +3830,11 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>chị Tiền</t>
+          <t>chị Lợi</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3855,10 +3855,10 @@
         <v/>
       </c>
       <c r="I88" t="n">
-        <v>10000000</v>
+        <v>1500000</v>
       </c>
       <c r="J88" t="n">
-        <v>5000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="89">
@@ -3868,11 +3868,11 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Như Tây</t>
+          <t>chị Tiền</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3896,7 +3896,7 @@
         <v>10000000</v>
       </c>
       <c r="J89" t="n">
-        <v>25000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="90">
@@ -3906,11 +3906,11 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Chị Xuyến</t>
+          <t>Như Tây</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3931,10 +3931,10 @@
         <v/>
       </c>
       <c r="I90" t="n">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="J90" t="n">
-        <v>4000000</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="91">
@@ -3944,11 +3944,11 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>em Nhi</t>
+          <t>Chị Xuyến</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3969,10 +3969,10 @@
         <v/>
       </c>
       <c r="I91" t="n">
-        <v>12000000</v>
+        <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="92">
@@ -3982,11 +3982,11 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Chị Loan</t>
+          <t>em Nhi</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4007,10 +4007,10 @@
         <v/>
       </c>
       <c r="I92" t="n">
-        <v>6000000</v>
+        <v>12000000</v>
       </c>
       <c r="J92" t="n">
-        <v>1000000</v>
+        <v>13000000</v>
       </c>
     </row>
     <row r="93">
@@ -4020,11 +4020,11 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Cô Trang</t>
+          <t>Chị Loan</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -4045,10 +4045,10 @@
         <v/>
       </c>
       <c r="I93" t="n">
+        <v>6000000</v>
+      </c>
+      <c r="J93" t="n">
         <v>1000000</v>
-      </c>
-      <c r="J93" t="n">
-        <v>3000000</v>
       </c>
     </row>
     <row r="94">
@@ -4058,11 +4058,11 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Trúc Thanh</t>
+          <t>Cô Trang</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -4083,10 +4083,10 @@
         <v/>
       </c>
       <c r="I94" t="n">
-        <v>5000000</v>
+        <v>1000000</v>
       </c>
       <c r="J94" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="95">
@@ -4096,25 +4096,23 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>C.Phượng</t>
+          <t>Trúc Thanh</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>SÓC TRĂNG</t>
+          <t>LONG XUYÊN</t>
         </is>
       </c>
       <c r="E95" t="n">
         <v/>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>0363094364</t>
-        </is>
+      <c r="F95" t="n">
+        <v/>
       </c>
       <c r="G95" t="n">
         <v/>
@@ -4123,10 +4121,10 @@
         <v/>
       </c>
       <c r="I95" t="n">
-        <v>7000000</v>
+        <v>5000000</v>
       </c>
       <c r="J95" t="n">
-        <v>6000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="96">
@@ -4136,11 +4134,11 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>c.Phiên</t>
+          <t>C.Phượng</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -4151,8 +4149,10 @@
       <c r="E96" t="n">
         <v/>
       </c>
-      <c r="F96" t="n">
-        <v/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>0363094364</t>
+        </is>
       </c>
       <c r="G96" t="n">
         <v/>
@@ -4161,10 +4161,10 @@
         <v/>
       </c>
       <c r="I96" t="n">
-        <v>5000000</v>
+        <v>7000000</v>
       </c>
       <c r="J96" t="n">
-        <v>1000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="97">
@@ -4174,11 +4174,11 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>c.Lan</t>
+          <t>c.Phiên</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -4199,10 +4199,10 @@
         <v/>
       </c>
       <c r="I97" t="n">
-        <v>15000000</v>
+        <v>5000000</v>
       </c>
       <c r="J97" t="n">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="98">
@@ -4212,11 +4212,11 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Lan Phương</t>
+          <t>c.Lan</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -4237,10 +4237,10 @@
         <v/>
       </c>
       <c r="I98" t="n">
-        <v>13000000</v>
+        <v>15000000</v>
       </c>
       <c r="J98" t="n">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="99">
@@ -4250,11 +4250,11 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>C.Hoành Ná</t>
+          <t>Lan Phương</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4275,10 +4275,10 @@
         <v/>
       </c>
       <c r="I99" t="n">
-        <v>2500000</v>
+        <v>13000000</v>
       </c>
       <c r="J99" t="n">
-        <v>1498000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="100">
@@ -4288,11 +4288,11 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Quan thị Hoa</t>
+          <t>C.Hoành Ná</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4313,10 +4313,10 @@
         <v/>
       </c>
       <c r="I100" t="n">
-        <v>0</v>
+        <v>2500000</v>
       </c>
       <c r="J100" t="n">
-        <v>10000000</v>
+        <v>1498000</v>
       </c>
     </row>
     <row r="101">
@@ -4326,16 +4326,16 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Lê Thị Nhanh</t>
+          <t>Quan thị Hoa</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>CẦN THƠ</t>
+          <t>SÓC TRĂNG</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -4351,10 +4351,10 @@
         <v/>
       </c>
       <c r="I101" t="n">
-        <v>17500000</v>
+        <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>9500000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="102">
@@ -4364,11 +4364,11 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Tường Vi</t>
+          <t>Lê Thị Nhanh</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4389,10 +4389,10 @@
         <v/>
       </c>
       <c r="I102" t="n">
-        <v>2000000</v>
+        <v>17500000</v>
       </c>
       <c r="J102" t="n">
-        <v>2000000</v>
+        <v>9500000</v>
       </c>
     </row>
     <row r="103">
@@ -4402,11 +4402,11 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Chị Đào</t>
+          <t>Tường Vi</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4427,10 +4427,10 @@
         <v/>
       </c>
       <c r="I103" t="n">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="J103" t="n">
-        <v>6000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="104">
@@ -4440,11 +4440,11 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Ngọc Hân</t>
+          <t>Chị Đào</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -4465,10 +4465,10 @@
         <v/>
       </c>
       <c r="I104" t="n">
-        <v>5000000</v>
+        <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>7000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="105">
@@ -4478,11 +4478,11 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Em Linh</t>
+          <t>Ngọc Hân</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4503,10 +4503,10 @@
         <v/>
       </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="J105" t="n">
-        <v>4000000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="106">
@@ -4516,36 +4516,74 @@
         </is>
       </c>
       <c r="B106" t="n">
+        <v>42</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Em Linh</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v/>
+      </c>
+      <c r="F106" t="n">
+        <v/>
+      </c>
+      <c r="G106" t="n">
+        <v/>
+      </c>
+      <c r="H106" t="n">
+        <v/>
+      </c>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>KH</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
         <v>41</v>
       </c>
-      <c r="C106" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t>Cẩm Tiên</t>
         </is>
       </c>
-      <c r="D106" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t>CẦN THƠ</t>
         </is>
       </c>
-      <c r="E106" t="n">
-        <v/>
-      </c>
-      <c r="F106" t="inlineStr">
+      <c r="E107" t="n">
+        <v/>
+      </c>
+      <c r="F107" t="inlineStr">
         <is>
           <t>0901279152</t>
         </is>
       </c>
-      <c r="G106" t="n">
-        <v/>
-      </c>
-      <c r="H106" t="n">
-        <v/>
-      </c>
-      <c r="I106" t="n">
+      <c r="G107" t="n">
+        <v/>
+      </c>
+      <c r="H107" t="n">
+        <v/>
+      </c>
+      <c r="I107" t="n">
         <v>16000000</v>
       </c>
-      <c r="J106" t="n">
+      <c r="J107" t="n">
         <v>2000000</v>
       </c>
     </row>

</xml_diff>